<commit_message>
Revision de plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1370 - HR, Enrique Peña Soto _MO/Planeación/Plan_proyecto.xlsx
+++ b/Proyectos/2015/12/P1370 - HR, Enrique Peña Soto _MO/Planeación/Plan_proyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,6 +31,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$22</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -1851,7 +1852,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D18 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -1986,8 +1987,8 @@
   </sheetPr>
   <dimension ref="A1:AMI30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4207,15 +4208,19 @@
         <v>42352</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="18" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="16" t="n">
+        <v>42348</v>
+      </c>
+      <c r="D18" s="16" t="n">
+        <v>42348</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A19" s="15"/>
@@ -4330,7 +4335,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="D18 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4547,6 +4552,27 @@
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
       <c r="E17" s="38"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39" t="s">
@@ -4594,7 +4620,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="D18 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4722,7 +4748,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="D18 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8990,7 +9016,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="D18 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9238,8 +9264,8 @@
   </sheetPr>
   <dimension ref="A1:JA41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="D18 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>